<commit_message>
Fix gene names in immunomodulatory annotation table
</commit_message>
<xml_diff>
--- a/tables/gene_annotations/immunomodulatory_genes.xlsx
+++ b/tables/gene_annotations/immunomodulatory_genes.xlsx
@@ -83,10 +83,13 @@
     <t xml:space="preserve">Cd274tm1(KOMP)Wtsi</t>
   </si>
   <si>
-    <t xml:space="preserve">ADORA2</t>
+    <t xml:space="preserve">ADORA2A</t>
   </si>
   <si>
     <t xml:space="preserve">Adora 2A receptor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADORA2</t>
   </si>
   <si>
     <t xml:space="preserve">CD276</t>
@@ -114,9 +117,6 @@
   </si>
   <si>
     <t xml:space="preserve">Icosltm1(KOMP)Wtsi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LGALS9</t>
   </si>
   <si>
     <t xml:space="preserve">LGALS9</t>
@@ -253,7 +253,7 @@
     <t xml:space="preserve">CD272</t>
   </si>
   <si>
-    <t xml:space="preserve">VISR</t>
+    <t xml:space="preserve">VSIR</t>
   </si>
   <si>
     <t xml:space="preserve">V-Set Domain-Containing Immunoregulatory Receptor</t>
@@ -277,7 +277,7 @@
     <t xml:space="preserve">regulation of B / T cell activation </t>
   </si>
   <si>
-    <t xml:space="preserve">IL6 </t>
+    <t xml:space="preserve">IL6</t>
   </si>
   <si>
     <t xml:space="preserve">induces acute inflammation </t>
@@ -925,7 +925,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4093,7 +4093,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>10</v>
@@ -5122,16 +5122,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>18</v>
@@ -6160,29 +6160,29 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
       <c r="J7" s="0"/>
       <c r="K7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M7" s="0"/>
       <c r="N7" s="0"/>
@@ -7202,7 +7202,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" s="0" t="s">
@@ -14466,7 +14466,7 @@
       </c>
       <c r="E15" s="0"/>
       <c r="F15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
@@ -16536,7 +16536,7 @@
         <v>53</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
@@ -61190,7 +61190,7 @@
         <v>149</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>150</v>
@@ -61271,7 +61271,7 @@
     </row>
     <row r="14" s="16" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>164</v>
@@ -61336,7 +61336,7 @@
         <v>171</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>18</v>

</xml_diff>